<commit_message>
Exported .svgs from model and added OWL file
</commit_message>
<xml_diff>
--- a/Rudder_Metamodel/CSRM Classes.xlsx
+++ b/Rudder_Metamodel/CSRM Classes.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahRudder\Documents\GitHub\CSRM--Rudder\Rudder_Metamodel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D9F416-44AC-4515-A2C5-ED882714A030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="103">
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>Documentation</t>
   </si>
@@ -369,13 +371,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -385,7 +386,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -402,430 +403,759 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="285" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:2" ht="399" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" ht="313.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:2" ht="384.75" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:2" ht="342" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:2" ht="370.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" ht="270.75" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:2" ht="327.75" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:2" ht="370.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:2" ht="384.75" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A50" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>